<commit_message>
create logic of category
</commit_message>
<xml_diff>
--- a/Robot_news_excel.xlsx
+++ b/Robot_news_excel.xlsx
@@ -462,17 +462,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Latinx small-business owners say a TikTok ban would cost them a valuable marketing platform — one that has had a tremendous impact on their ventures.</t>
+          <t>USC has left its valedictorian out in the cold, says one reader. Another believes the university failed to do its due diligence in the first place.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://ca-times.brightspotcdn.com/dims4/default/7cfd5d1/2147483647/strip/true/crop/1080x720+0+195/resize/840x560!/quality/75/?url=https%3A%2F%2Fcalifornia-times-brightspot.s3.amazonaws.com%2Fe4%2F85%2F69d091b04125841dc090f415b2ee%2Ftiktok-1.png</t>
+          <t>https://ca-times.brightspotcdn.com/dims4/default/718115b/2147483647/strip/true/crop/4417x2945+0+0/resize/840x560!/quality/75/?url=https%3A%2F%2Fcalifornia-times-brightspot.s3.amazonaws.com%2F15%2F90%2F1e353fe8420ca44bfd0d9fdcc2dd%2F958583-me-usc-commencement-jja-0016.jpg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>47 minutes ago</t>
+          <t>1 hour ago</t>
         </is>
       </c>
       <c r="E2" t="b">

</xml_diff>